<commit_message>
TC Sprint 37 (Modificaciones en Archivo Debin) TC regresion Release 224 (Modificaciones en Archivo Garantia Liquidaciones) ID TC DebinQR
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - Escenarios y Casos de Pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E844F673-62CC-4790-99EB-9DA3B55AA79E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325155FF-115C-4620-A718-71814C55A772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="113">
   <si>
     <t>Parametros</t>
   </si>
@@ -334,6 +334,45 @@
   </si>
   <si>
     <t>CONTRACARGO DESTINO Y ORIGEN CVU - 5559 - RECURRENCIA NO ENCONTRADA, ERROR DE DATOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debin Recurrente CVU - Validar Error Fallan Garantías </t>
+  </si>
+  <si>
+    <t>CashOut*</t>
+  </si>
+  <si>
+    <t>CASHOUT - Validación ori_trx_id - CBU &gt; CBU</t>
+  </si>
+  <si>
+    <t>{"StatusCode":200,"Mensaje":{"respuesta": {"codigo":"7552","descripcion":"8PDX4OGNYJ0P80VN0L6EY5 - ID DE OPERACION  EXISTENTE"}}}</t>
+  </si>
+  <si>
+    <t>"objeto":{"tipo":"CASHOUT","ori_trx_id":1126},"credito":{"cuit":"20000014479","banco":"998","sucursal":"8851","cuenta":{"cbu":"0000004800000000014485"},"titular":""},"debito":{"cuit":"27956331957","banco":"000","sucursal":"0161","cuenta":{"cbu":"0000161400000000004309"},"titular":"PRUEBAS COELSA CASHOUT"},"importe":{"importe":10}}</t>
+  </si>
+  <si>
+    <t>"objeto":{"tipo":"CASHOUT","ori_trx_id":1127},"credito":{"cuit":"20333048494","banco":"998","sucursal":"8851","cuenta":{"cbu":"9988851800000000000628"},"titular":""},"debito":{"cuit":"20000009963","banco":"000","sucursal":"0161","cuenta":{"cbu":"9984788700000000000420"},"titular":"PRUEBAS COELSA CASHOUT"},"importe":{"importe":10}}</t>
+  </si>
+  <si>
+    <t>{"StatusCode":200,"Mensaje":{"respuesta": {"codigo":"7552","descripcion":"PD4RO172V1XQWXR9KJ3QE6 - ID DE OPERACION  EXISTENTE"}}}</t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"cuit":"20000014479","cbu":"0000004800000000014485","banco":"998","recurrencia":true,"prestacion":"AutomationMVP3"},"comprador":{"cuit":"27956331957","cuenta":{"cbu":"0000161400000000004309","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":9999999.01}}}|"operacion":{"comprador":{"cuit":"27956331957","cuenta":{"cbu":"0000161400000000004309"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":9999999.01}}}|"operacion":{"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":9999999.01}}}</t>
+  </si>
+  <si>
+    <t>{"StatusCode":200,"Mensaje":{"codigo": "31", "descripcion": "EL BANCO DE DEBITO NO POSEE GARANTIAS SUFICIENTES"}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CASHOUT - Validación ori_trx_id - CVU &gt; CVU </t>
+  </si>
+  <si>
+    <t>{"StatusCode":200,"Mensaje":{"respuesta": {"codigo":"7541","descripcion":"PERSISTIDO"}}}</t>
+  </si>
+  <si>
+    <t>CASHOUT - AvisoCredito - Tipo de objeto 'CASHOUT'</t>
+  </si>
+  <si>
+    <t>"objeto":{"tipo":"CASHOUT"},"credito":{"cuit":"20956746117","banco":"000","sucursal":"0213","cuenta":{"cbu":"0000213699900070000000"},"titular":""},"debito":{"cuit":"20333048494","banco":"998","sucursal":"8851","cuenta":{"cbu":"9988851800000000000628"},"titular":"PRUEBAS COELSA CASHOUT"},"importe":{"importe":10}}</t>
   </si>
 </sst>
 </file>
@@ -688,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63218BCB-F1F0-4D18-A551-3DB8181D382F}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,20 +1083,20 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="10" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
+    <row r="21" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
         <v>53096</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1129,20 +1168,20 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="10" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A26" s="9">
+    <row r="26" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
         <v>53104</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="13" t="s">
+      <c r="E26" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1346,7 +1385,7 @@
       <c r="D38" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" s="6" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1363,9 +1402,82 @@
       <c r="D39" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="6" t="s">
         <v>95</v>
       </c>
+    </row>
+    <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>59007</v>
+      </c>
+      <c r="B40" t="s">
+        <v>101</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A41" s="9">
+        <v>59006</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A42" s="9">
+        <v>59199</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="9">
+        <v>59305</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
cambio de datos en archivos Excel
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - Escenarios y Casos de Pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCCCEB3-28CF-4CA2-9C94-84AD675D4616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B060A299-40D5-4CFC-AF34-B13AA4181944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="134">
   <si>
     <t>Parametros</t>
   </si>
@@ -191,9 +191,6 @@
     <t>"operacion":{"vendedor":{"cuit":"20000000222","cbu":"9981522200000000000192","banco":"998","recurrencia":true},"comprador":{"cuit":"20000001008","cuenta":{"cbu":"0000210500200000010083","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":120}}}</t>
   </si>
   <si>
-    <t>"operacion":{"vendedor":{"cuit":"20333048494","cbu":"9988851800000000000628","banco":"998","recurrencia":true,"prestacion":"Garantia"},"comprador":{"cuit":"27956331957","cuenta":{"cbu":"0000161400000000004309","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":360}}}|"operacion":{"comprador":{"cuit":"27956331957","cuenta":{"cbu":"0000161400000000004309"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":360}}}|"operacion":{"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":360}}}</t>
-  </si>
-  <si>
     <t>CONTRACARGO DESTINO Y ORIGEN CVU - Solicitar al Vendedor la devolución</t>
   </si>
   <si>
@@ -257,18 +254,6 @@
     <t>"operacion":{"vendedor":{"cuit":"20333048494","cbu":"00000017000000000084","banco":"000","recurrencia":true,"prestacion":"MVP2"},"comprador":{"cuit":"20000000222","cuenta":{"cbu":"0000207500000000000055","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":490}}}</t>
   </si>
   <si>
-    <t>"operacion":{"vendedor":{"cuit":"20000014479","cbu":"0000004800000000014485","banco":"000","recurrencia":true,"prestacion":"AutomationMVP3"},"comprador":{"cuit":"27956331957","cuenta":{"cbu":"0000161400000000004309","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":400}}}|"operacion":{"comprador":{"cuit":"27956331957","cuenta":{"cbu":"0000161400000000004309"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":400}},"respuesta":{"codigo":"88"}}</t>
-  </si>
-  <si>
-    <t>"operacion":{"vendedor":{"cuit":"20000014479","cbu":"0000004800000000014485","banco":"000","recurrencia":true,"prestacion":"AutomationMVP3"},"comprador":{"cuit":"27956331957","cuenta":{"cbu":"0000161400000000004309","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":360}}}|"operacion":{"comprador":{"cuit":"27956331957","cuenta":{"cbu":"0000161400000000004309"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":360}}}|"operacion":{"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":360}},"respuesta":{"codigo":"88"}}</t>
-  </si>
-  <si>
-    <t>"operacion":{"vendedor":{"cuit":"20000014479","cbu":"0000004800000000014485","banco":"000","recurrencia":true,"prestacion":"AutomationMVP3"},"comprador":{"cuit":"27956331957","cuenta":{"cbu":"0000161400000000004309","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":999999999999}}}|"operacion":{"comprador":{"cuit":"27956331957","cuenta":{"cbu":"0000161400000000004309"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":999999999999}}}|"operacion":{"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":999999999999}}}</t>
-  </si>
-  <si>
-    <t>"operacion":{"vendedor":{"cuit":"20000014479","cbu":"0000004800000000014485","banco":"000","recurrencia":true,"prestacion":"AutomationMVP3"},"comprador":{"cuit":"27956331957","cuenta":{"cbu":"0000161400000000004309","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":999999999999,}}}|"operacion":{"comprador":{"cuit":"27956331957","cuenta":{"cbu":"0000161400000000004309"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":999999999999,}}}|"operacion":{"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":999999999999,}},"respuesta":{"codigo":"88"}}</t>
-  </si>
-  <si>
     <t>"operacion":{"vendedor":{"cuit":"20000014479","cbu":"0000004800000000014485","banco":"000","recurrencia":true,"prestacion":"AutomationMVP3"},"comprador":{"cuit":"27956331957","cuenta":{"cbu":"0000161400000000004309","alias":""}},"detalle":{"importe":360}}}|"operacion":{"comprador":{"cuit":"27956331957","cuenta":{"cbu":"0000161400000000004309"}},"detalle":{"importe":360}}}|"operacion":{"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420"}},"detalle":{"ori_trx":"00000307","importe":360}}}|"operacionOriginal":{"detalle":{"importe":360}},"comprador":{"cuit":"27956331957","cuenta":{"cbu":"0000161400000000004309"}},"vendedor":{"cuit":"20000014479","cuenta":{"cbu":"0000004800000000014485"}}}</t>
   </si>
   <si>
@@ -293,21 +278,12 @@
     <t>"operacion":{"vendedor":{"cuit":"20000001008","cbu":"0000210500200000010083","banco":"000"},"comprador":{"cuit":"20000000222","cuenta":{"cbu":"9981522200000000000192","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":300.02}}}|"operacion":{"comprador":{"cuit":"20000000222","cuenta":{"cbu":"9981522200000000000192"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":300.02}}}</t>
   </si>
   <si>
-    <t>"operacion":{"vendedor":{"cuit":"27956331957","cbu":"0000004800000000114208","banco":"000"},"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":400}}}|"operacion":{"comprador":{"cuit":"27956331957","cuenta":{"cbu":"0000161400000000004309"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":400}},"respuesta":{"codigo":"88"}}</t>
-  </si>
-  <si>
-    <t>"operacion":{"vendedor":{"cuit":"27956331957","cbu":"0000004800000000114208","banco":"000"},"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":420,"devolucion":true,"tiempoExpiracion":360,"descripción":"MVP2","mismoTitular":0},"datosGenerador":{"ipCliente":"","tipoDispositivo":"","plataforma":"","imsi":"","imei":"","ubicacion":{"lat":0,"lng":0,"precision":0}}}}|"operacion":{"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":420}},"respuesta":{"codigo":"88"}}</t>
-  </si>
-  <si>
     <t>"operacion":{"vendedor":{"cuit":"20000001008","cbu":"0000210500200000010083","banco":"000"},"comprador":{"cuit":"23202020208","cuenta":{"cbu":"0000210500000000212452","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":360}}}|"operacion":{"comprador":{"cuit":"23202020208","cuenta":{"cbu":"0000210500000000212452"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":360}}}</t>
   </si>
   <si>
     <t>"operacion":{"vendedor":{"cuit":"20000001008","cbu":"0000210500200000010083","banco":"000"},"comprador":{"cuit":"23202020208","cuenta":{"cbu":"0000210500000000212452","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":360}}}|"operacion":{"comprador":{"cuit":"23202020208","cuenta":{"cbu":"0000210500000000212452"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":360}}}|"operacion":{"comprador":{"cuit":"23000009989","cuenta":{"cbu":"9985340400000000000529"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":360}}}</t>
   </si>
   <si>
-    <t>"operacion":{"vendedor":{"cuit":"27956331957","cbu":"0000004800000000114208","banco":"000"},"comprador":{"cuit":"23202020208","cuenta":{"cbu":"0000210500000000212452","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":110}}}|"operacion":{"comprador":{"cuit":"23202020208","cuenta":{"cbu":"0000210500000000212452"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":110}},"respuesta":{"codigo":"88"}}</t>
-  </si>
-  <si>
     <t>"operacion":{"vendedor":{"cuit":"20000001008","cbu":"0000210500200000010083","banco":"000"},"comprador":{"cuit":"23202020208","cuenta":{"cbu":"0000210500000000212452","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":150}}}|"operacion":{"comprador":{"cuit":"23202020208","cuenta":{"cbu":"0000210500000000212452"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":150}}}|"operacion":{"comprador":{"cuit":"23000009989","cuenta":{"cbu":"9985340400000000000529"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":150}},"respuesta":{"codigo":"88"}}</t>
   </si>
   <si>
@@ -320,21 +296,9 @@
     <t>"operacion":{"vendedor":{"cuit":"200000144","cbu":"0000004800000000014485","banco":"000","recurrencia":true,"prestacion":"SivENDE"},"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":170}}}</t>
   </si>
   <si>
-    <t>"operacion":{"vendedor":{"cuit":"20000014479","cbu":"0000004800000000014485","banco":"000","recurrencia":true,"prestacion":"SivENDE"},"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":400}}}|"operacion":{"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":400}},"respuesta":{"codigo":"88"}}</t>
-  </si>
-  <si>
-    <t>"operacion":{"vendedor":{"cuit":"20000014479","cbu":"0000004800000000014485","banco":"000","recurrencia":true,"prestacion":"SivENDE"},"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420"}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":420}}}|"operacion":{"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":420}},"respuesta":{"codigo":"88"}}</t>
-  </si>
-  <si>
     <t>"operacion":{"vendedor":{"cuit":"20333048494","cbu":"0000001700000000008455","banco":"000","recurrencia":true,"prestacion":"MVP2"},"comprador":{"cuit":"20000000222","cuenta":{"cbu":"0000207500000000000055","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":790}}}</t>
   </si>
   <si>
-    <t>"operacion":{"vendedor":{"cuit":"20000014479","cbu":"0000004800000000014485","banco":"000","recurrencia":true,"prestacion":"AutomationMVP3"},"comprador":{"cuit":"27956331957","cuenta":{"cbu":"0000161400000000004309","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":360}}}|"operacion":{"comprador":{"cuit":"27956331957","cuenta":{"cbu":"0000161400000000004309"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":360}}}</t>
-  </si>
-  <si>
-    <t>"operacion":{"vendedor":{"cuit":"20000014479","cbu":"0000004800000000014485","banco":"000","recurrencia":true,"prestacion":"AutomationMVP3"},"comprador":{"cuit":"27956331957","cuenta":{"cbu":"0000161400000000004309","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":360}}}|"operacion":{"comprador":{"cuit":"27956331957","cuenta":{"cbu":"0000161400000000004309"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":360}}}|"operacion":{"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":360}}}</t>
-  </si>
-  <si>
     <t>Debin Recurrente CVU&gt;CVU - Crear Debin - Recaudadora Inactiva del Vendedor</t>
   </si>
   <si>
@@ -356,9 +320,6 @@
     <t>"operacion":{"vendedor":{"cuit":"20333048494","cbu":"9988851800000000000628","banco":"998","recurrencia":true,"prestacion":"PRESTACION23456"},"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":199.02}}}|"operacion":{"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":199.02}}}|"id":"debin.id"</t>
   </si>
   <si>
-    <t>"operacion":{"vendedor":{"cuit":"20000014479","cbu":"0000004800000000014485","banco":"000","recurrencia":true,"prestacion":"SivENDE"},"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":175.02}}}|"operacion":{"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":175.02}}}</t>
-  </si>
-  <si>
     <t>"operacion":{"vendedor":{"cuit":"20333048494","cbu":"9988851800000000000628","banco":"998","recurrencia":true,"prestacion":"PRESTACION23456"},"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":199.02}}}|"operacion":{"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":199.02}}}</t>
   </si>
   <si>
@@ -435,6 +396,54 @@
   </si>
   <si>
     <t>"operacion":{"detalle":{"concepto":"ECT","importe":1000}}}|"operacion":{"comprador":{"cuit":"23000009989","cuenta":{"cbu":"9985340400000000000529"}},"detalle":{"ori_terminal":"","ori_adicional":"","moneda":"032","importe":1000}}}|"id":"debin.id"|"aviso":"QrConfirmaDebito","producto":"responder"</t>
+  </si>
+  <si>
+    <t>"id":"M67REZ8NP1E64ZG24KVGOP"</t>
+  </si>
+  <si>
+    <t>debindebin4*</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ​GET /apiDebinV1​/Debin​/Debin4​/{id} - Funcionamiento correcto </t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"cuit":"20000001008","cbu":"0000210500200000010083","banco":"000"},"comprador":{"cuit":"23202020208","cuenta":{"cbu":"0000210500000000212452","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":110}}}|"operacion":{"comprador":{"cuit":"23202020208","cuenta":{"cbu":"0000210500000000212452"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":110}},"respuesta":{"codigo":"88"}}</t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"cuit":"20000001008","cbu":"0000210500200000010083","banco":"000","recurrencia":true,"prestacion":"PrestacionAUT"},"comprador":{"cuit":"23202020208","cuenta":{"cbu":"0000210500000000212452","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":360}}}|"operacion":{"comprador":{"cuit":"23202020208","cuenta":{"cbu":"0000210500000000212452"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":360}}}</t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"cuit":"20000001008","cbu":"0000210500200000010083","banco":"000","recurrencia":true,"prestacion":"PrestacionAUT"},"comprador":{"cuit":"23202020208","cuenta":{"cbu":"0000210500000000212452","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":400}}}|"operacion":{"comprador":{"cuit":"23202020208","cuenta":{"cbu":"0000210500000000212452"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":400}},"respuesta":{"codigo":"88"}}</t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"cuit":"20000001008","cbu":"0000210500200000010083","banco":"000"},"comprador":{"cuit":"23202020208","cuenta":{"cbu":"0000210500000000212452","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":400}}}|"operacion":{"comprador":{"cuit":"23000009989","cuenta":{"cbu":"9985340400000000000529"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":400}},"respuesta":{"codigo":"88"}}</t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"cuit":"20000001008","cbu":"0000210500200000010083","banco":"000","recurrencia":true,"prestacion":"PrestacionAUTCBU"},"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":400}}}|"operacion":{"comprador":{"cuit":"2000000|9963","cuenta":{"cbu":"9984788700000000000420"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":400}},"respuesta":{"codigo":"88"}}</t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"cuit":"20000001008","cbu":"0000210500200000010083","banco":"000"},"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":420,"devolucion":true,"tiempoExpiracion":360,"descripción":"PrestacionAUTCBU","mismoTitular":0},"datosGenerador":{"ipCliente":"","tipoDispositivo":"","plataforma":"","imsi":"","imei":"","ubicacion":{"lat":0,"lng":0,"precision":0}}}}|"operacion":{"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":420}},"respuesta":{"codigo":"88"}}</t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"cuit":"20000001008","cbu":"0000210500200000010083","banco":"000","recurrencia":true,"prestacion":"PrestacionAUTCBU"},"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":175.02}}}|"operacion":{"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":175.02}}}</t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"cuit":"20000001008","cbu":"0000210500200000010083","banco":"000","recurrencia":true,"prestacion":"PrestacionAUTCBU"},"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420"}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":420}}}|"operacion":{"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":420}},"respuesta":{"codigo":"88"}}</t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"cuit":"20000001008","cbu":"0000210500200000010083","banco":"000","recurrencia":true,"prestacion":"PrestacionAUT"},"comprador":{"cuit":"23202020208","cuenta":{"cbu":"0000210500000000212452","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":360}}}|"operacion":{"comprador":{"cuit":"23202020208","cuenta":{"cbu":"0000210500000000212452"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":360}}}|"operacion":{"comprador":{"cuit":"23000009989","cuenta":{"cbu":"9985340400000000000529"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":360}}}</t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"cuit":"20000001008","cbu":"0000210500200000010083","banco":"000","recurrencia":true,"prestacion":"PrestacionAUT"},"comprador":{"cuit":"23202020208","cuenta":{"cbu":"0000210500000000212452","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":360}}}|"operacion":{"comprador":{"cuit":"23202020208","cuenta":{"cbu":"0000210500000000212452"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":360}}}|"operacion":{"comprador":{"cuit":"23000009989","cuenta":{"cbu":"9985340400000000000529"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":360}},"respuesta":{"codigo":"88"}}</t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"cuit":"20000001008","cbu":"0000210500200000010083","banco":"000","recurrencia":true,"prestacion":"PrestacionAUT"},"comprador":{"cuit":"23202020208","cuenta":{"cbu":"0000210500000000212452","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":999999999999}}}|"operacion":{"comprador":{"cuit":"23202020208","cuenta":{"cbu":"0000210500000000212452"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":999999999999}}}|"operacion":{"comprador":{"cuit":"23000009989","cuenta":{"cbu":"9985340400000000000529"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":999999999999}}}</t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"cuit":"20000001008","cbu":"0000210500200000010083","banco":"000","recurrencia":true,"prestacion":"PrestacionAUT"},"comprador":{"cuit":"23202020208","cuenta":{"cbu":"0000210500000000212452","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":999999999999,}}}|"operacion":{"comprador":{"cuit":"23202020208","cuenta":{"cbu":"0000210500000000212452"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":999999999999,}}}|"operacion":{"comprador":{"cuit":"23000009989","cuenta":{"cbu":"9985340400000000000529"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":999999999999,}},"respuesta":{"codigo":"88"}}</t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"cuit":"20333048494","cbu":"9988851800000000000628","banco":"998","recurrencia":true,"prestacion":"PrestacionAUTCBU2"},"comprador":{"cuit":"23202020208","cuenta":{"cbu":"0000210500000000212452","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":360}}}|"operacion":{"comprador":{"cuit":"23202020208","cuenta":{"cbu":"0000210500000000212452"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":360}}}|"operacion":{"comprador":{"cuit":"23000009989","cuenta":{"cbu":"9985340400000000000529"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":360}}}</t>
   </si>
 </sst>
 </file>
@@ -791,7 +800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63218BCB-F1F0-4D18-A551-3DB8181D382F}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView topLeftCell="D7" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E12"/>
     </sheetView>
   </sheetViews>
@@ -830,7 +839,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>36</v>
@@ -847,13 +856,13 @@
         <v>5</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -864,13 +873,13 @@
         <v>5</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -881,7 +890,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>36</v>
@@ -898,7 +907,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>36</v>
@@ -915,7 +924,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>44</v>
@@ -932,7 +941,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>45</v>
@@ -949,7 +958,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>36</v>
@@ -966,7 +975,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>45</v>
@@ -983,7 +992,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>44</v>
@@ -1019,8 +1028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F36B566-A8B3-4276-BF15-5382541B3162}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A2:A7"/>
+    <sheetView topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1058,7 +1067,7 @@
         <v>37</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>83</v>
+        <v>124</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>39</v>
@@ -1075,7 +1084,7 @@
         <v>37</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>41</v>
@@ -1092,7 +1101,7 @@
         <v>37</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>87</v>
+        <v>121</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>38</v>
@@ -1109,7 +1118,7 @@
         <v>37</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>39</v>
@@ -1126,7 +1135,7 @@
         <v>37</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>41</v>
@@ -1143,7 +1152,7 @@
         <v>37</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>71</v>
+        <v>123</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>38</v>
@@ -1162,8 +1171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE05897-A124-4DF1-94F7-2D87CB9F2977}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,7 +1210,7 @@
         <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>40</v>
@@ -1218,7 +1227,7 @@
         <v>35</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>84</v>
+        <v>126</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>38</v>
@@ -1252,7 +1261,7 @@
         <v>43</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>40</v>
@@ -1269,7 +1278,7 @@
         <v>43</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>38</v>
@@ -1295,7 +1304,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>53137</v>
       </c>
@@ -1303,7 +1312,7 @@
         <v>35</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>40</v>
@@ -1320,7 +1329,7 @@
         <v>35</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>40</v>
@@ -1337,7 +1346,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>93</v>
+        <v>128</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>38</v>
@@ -1354,7 +1363,7 @@
         <v>43</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>96</v>
+        <v>129</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>40</v>
@@ -1371,7 +1380,7 @@
         <v>43</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>49</v>
+        <v>133</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>40</v>
@@ -1380,7 +1389,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>53106</v>
       </c>
@@ -1388,7 +1397,7 @@
         <v>43</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>72</v>
+        <v>130</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>38</v>
@@ -1405,7 +1414,7 @@
         <v>43</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>73</v>
+        <v>131</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>47</v>
@@ -1422,7 +1431,7 @@
         <v>43</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>74</v>
+        <v>132</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>38</v>
@@ -1436,16 +1445,16 @@
         <v>61354</v>
       </c>
       <c r="B16" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1453,16 +1462,16 @@
         <v>61938</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1470,16 +1479,16 @@
         <v>62083</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1487,16 +1496,16 @@
         <v>62085</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1504,13 +1513,13 @@
         <v>61417</v>
       </c>
       <c r="B20" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="E20" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1518,13 +1527,13 @@
         <v>61485</v>
       </c>
       <c r="B21" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="E21" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1532,7 +1541,7 @@
         <v>61487</v>
       </c>
       <c r="E22" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1540,7 +1549,7 @@
         <v>61944</v>
       </c>
       <c r="E23" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1548,7 +1557,7 @@
         <v>61945</v>
       </c>
       <c r="E24" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1600,16 +1609,16 @@
         <v>54148</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="105" x14ac:dyDescent="0.25">
@@ -1617,16 +1626,16 @@
         <v>54157</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="105" x14ac:dyDescent="0.25">
@@ -1634,16 +1643,16 @@
         <v>54175</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="105" x14ac:dyDescent="0.25">
@@ -1651,16 +1660,16 @@
         <v>54177</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="105" x14ac:dyDescent="0.25">
@@ -1668,16 +1677,16 @@
         <v>54181</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
@@ -1685,16 +1694,16 @@
         <v>54272</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="105" x14ac:dyDescent="0.25">
@@ -1702,16 +1711,16 @@
         <v>55448</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="135" x14ac:dyDescent="0.25">
@@ -1719,16 +1728,16 @@
         <v>55449</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="135" x14ac:dyDescent="0.25">
@@ -1736,16 +1745,16 @@
         <v>54359</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1756,10 +1765,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E10034F-8FD9-4FCB-9336-0FB21B23CB37}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1794,16 +1803,16 @@
         <v>58877</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1811,14 +1820,28 @@
         <v>60588</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C3" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="6" t="s">
-        <v>107</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>62555</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
otro cambios en archivos de excel
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - Escenarios y Casos de Pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2321E04-FC6F-485B-8551-A4D0482955C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C42792E-102F-4EFB-B089-A99E9DF2C5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -452,13 +452,13 @@
     <t>Modificar GET /apiDebinV1​/Debin​/Debin3/{ori_trx_id} - ID HASH inexistente</t>
   </si>
   <si>
-    <t>"debin.ori_trx_id":"12347"</t>
-  </si>
-  <si>
-    <t>"debin.ori_trx_id":"9223000000000"</t>
-  </si>
-  <si>
-    <t>"debin.ori_trx_id":"9223000000000066168"</t>
+    <t>"ori_trx_id":"12347"</t>
+  </si>
+  <si>
+    <t>"ori_trx_id":"9223000000000"</t>
+  </si>
+  <si>
+    <t>"ori_trx_id":"9223000000000066168"</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
nuevos TCs metodo debin y debinQR
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - Escenarios y Casos de Pruebas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C42792E-102F-4EFB-B089-A99E9DF2C5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832CB647-0CB1-4541-9A39-A3C2CCB350D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Debin" sheetId="7" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="145">
   <si>
     <t>Parametros</t>
   </si>
@@ -459,6 +459,24 @@
   </si>
   <si>
     <t>"ori_trx_id":"9223000000000066168"</t>
+  </si>
+  <si>
+    <t>Debin*-&gt;debindebin2*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get Debin 2 --&gt; consultar por un Debin </t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"cuit":"20333048494","cbu":"9988851800000000000628","banco":"998","recurrencia":true,"prestacion":"PRESTACION23456"},"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420","alias":""}},"detalle":{"concepto":"PCT","idUsuario":11232,"idComprobante":922808,"moneda":"032","importe":199.02}}}|"id":"debin.id"</t>
+  </si>
+  <si>
+    <t>Credito*-&gt;debindebin2*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get Debin 2 --&gt; consultar por una Transferencia </t>
+  </si>
+  <si>
+    <t>"umbral_riesgo":100,"debito":{"cuit":"20000009998","banco":"998","sucursal":"0547","cuenta":{"cbu":"9980547400000000000055"},"titular":"string"},"credito":{"cuit":"23076812179","banco":"415","sucursal":"0999","cuenta":{"cbu":"4150999718001586640025"},"titular":"string"},"concepto":"VAR"}|"id":"debin.id"</t>
   </si>
 </sst>
 </file>
@@ -1773,10 +1791,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E10034F-8FD9-4FCB-9336-0FB21B23CB37}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1848,7 +1866,7 @@
       <c r="C4" t="s">
         <v>102</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="6" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1862,7 +1880,7 @@
       <c r="C5" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="6" t="s">
         <v>133</v>
       </c>
     </row>
@@ -1876,7 +1894,7 @@
       <c r="C6" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="6" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1893,8 +1911,39 @@
       <c r="D7" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="6" t="s">
         <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>53393</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>53396</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nuevo campo en deinQ
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - Escenarios y Casos de Pruebas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832CB647-0CB1-4541-9A39-A3C2CCB350D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BC76F1-E621-463B-87E9-2B12CC5A8B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Debin" sheetId="7" r:id="rId1"/>
@@ -850,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63218BCB-F1F0-4D18-A551-3DB8181D382F}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F36B566-A8B3-4276-BF15-5382541B3162}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1221,8 +1221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE05897-A124-4DF1-94F7-2D87CB9F2977}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView topLeftCell="B17" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1794,7 +1794,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
un TCS de un get
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - Escenarios y Casos de Pruebas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BC76F1-E621-463B-87E9-2B12CC5A8B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B902E2D5-45A8-47A5-A964-06093486A81B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Debin" sheetId="7" r:id="rId1"/>
@@ -1599,7 +1599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10450D68-B822-44A3-8B40-94E2DA131214}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1793,8 +1793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E10034F-8FD9-4FCB-9336-0FB21B23CB37}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
acciones y semillas nuevas de refunds y payments bcraid, nuevos casos del sprint 41 (debinqr, refunds y payment)
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - Escenarios y Casos de Pruebas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B220D1-1264-42AD-A7B9-F16D576AA9CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900CDC80-C1D0-4871-BDC9-D573993F4906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Debin" sheetId="7" r:id="rId1"/>
@@ -1622,7 +1622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10450D68-B822-44A3-8B40-94E2DA131214}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -1821,7 +1821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E10034F-8FD9-4FCB-9336-0FB21B23CB37}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
pequeños cambios en archivos de excel
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - Escenarios y Casos de Pruebas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900CDC80-C1D0-4871-BDC9-D573993F4906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B05BFC-4164-4DFC-81C6-DF1A62DCD1D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Debin" sheetId="7" r:id="rId1"/>
@@ -470,9 +470,6 @@
     <t>"operacion":{"vendedor":{"recurrencia":true,"prestacion":"PrestacionAUT"},"detalle":{"importe":360}}}|"operacion":{"detalle":{"importe":360}}}|"operacion":{"detalle":{"importe":360}}}|"operacionOriginal":{"detalle":{"importe":360}}}|"operacionOriginal":{"detalle":{"importe":360}},"vendedor":{"cuit":"2000000100","cuenta":{"cbu":"0000210500200000010083"}}}</t>
   </si>
   <si>
-    <t>"operacion":{"vendedor":{"cuit":"20000009963","cbu":"9984788700000000000420","banco":"998","recurrencia":true,"prestacion":"AUTCBU2"},"comprador":{"cuit":"23202020208","cuenta":{"cbu":"0000210500000000212452","alias":""}},"detalle":{"importe":230}}}|"operacion":{"comprador":{"cuit":"23202020208","cuenta":{"cbu":"0000210500000000212452"}},"detalle":{"ori_trx":"00000307","ori_terminal":"","ori_adicional":"","moneda":"032","importe":230}}}|"operacion":{"comprador":{"cuit":"23000009989","cuenta":{"cbu":"9985340400000000000529"}},"detalle":{"importe":230}}}|"operacionOriginal":{"detalle":{"importe":230}},"comprador":{"cuit":"23202020208","cuenta":{"cbu":"0000210500000000212452"}},"vendedor":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420"}}}</t>
-  </si>
-  <si>
     <t>"operacion":{"detalle":{"concepto":"ECT","importe":1000}}}|"operacion":{"comprador":{"cuit":"23000009989","cuenta":{"cbu":"9985340400000000000529"}},"detalle":{"ori_terminal":"","ori_adicional":"","moneda":"032","importe":1000}}}|"id":"debin.id","aviso":"QRIntencionPago","producto":"responder"</t>
   </si>
   <si>
@@ -486,6 +483,9 @@
   </si>
   <si>
     <t>"oritrxid":"9223000000000"</t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"cuit":"23200000021","cbu":"9981405210000000110029","banco":"998","recurrencia":true,"prestacion":"Mollejito"},"detalle":{"importe":230}}|"operacion":{"detalle":{"importe":230}}}|"operacion":{"detalle":{"importe":230}}}|"operacionOriginal":{"detalle":{"importe":230}},"vendedor":{"cuit":"23200000021","cuenta":{"cbu":"9981405210000000110029"}}}</t>
   </si>
 </sst>
 </file>
@@ -501,18 +501,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -527,7 +521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -554,17 +548,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -859,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63218BCB-F1F0-4D18-A551-3DB8181D382F}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,7 +1071,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,8 +1213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE05897-A124-4DF1-94F7-2D87CB9F2977}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1603,10 +1586,10 @@
         <v>99</v>
       </c>
       <c r="C22" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1622,8 +1605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10450D68-B822-44A3-8B40-94E2DA131214}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1772,20 +1755,20 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
+    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <v>55449</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="D9" s="14" t="s">
+      <c r="C9" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="6" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1821,8 +1804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E10034F-8FD9-4FCB-9336-0FB21B23CB37}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1906,7 +1889,7 @@
         <v>125</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>126</v>
@@ -1920,7 +1903,7 @@
         <v>125</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>127</v>
@@ -1934,7 +1917,7 @@
         <v>125</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>124</v>

</xml_diff>